<commit_message>
Saved so it doc opens on first sheet
</commit_message>
<xml_diff>
--- a/VCP6.5 DCV Study Tracker.xlsx
+++ b/VCP6.5 DCV Study Tracker.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="9945" tabRatio="674" firstSheet="4" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="9945" tabRatio="674"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -8239,7 +8239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -8828,7 +8828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1:K25"/>
     </sheetView>

</xml_diff>

<commit_message>
Formatting on Summary sheet
</commit_message>
<xml_diff>
--- a/VCP6.5 DCV Study Tracker.xlsx
+++ b/VCP6.5 DCV Study Tracker.xlsx
@@ -8237,10 +8237,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8361,40 +8361,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
+      <c r="B16" s="23"/>
+    </row>
+    <row r="17" spans="1:1" ht="210" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
         <v>384</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>379</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>380</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A21" r:id="rId1"/>
-    <hyperlink ref="A22" r:id="rId2"/>
+    <hyperlink ref="A22" r:id="rId1"/>
+    <hyperlink ref="A23" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Removed values from topics with sub topics
</commit_message>
<xml_diff>
--- a/VCP6.5 DCV Study Tracker.xlsx
+++ b/VCP6.5 DCV Study Tracker.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="9945" tabRatio="674" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="9945" tabRatio="674" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -8554,7 +8554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -10597,9 +10597,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10758,9 +10758,7 @@
       <c r="A19" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="B19" s="8">
-        <v>0</v>
-      </c>
+      <c r="B19" s="8"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
@@ -10814,9 +10812,7 @@
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="8">
-        <v>0</v>
-      </c>
+      <c r="B26" s="8"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
@@ -11006,9 +11002,7 @@
       <c r="A50" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B50" s="8">
-        <v>0</v>
-      </c>
+      <c r="B50" s="8"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
@@ -11038,9 +11032,7 @@
       <c r="A54" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B54" s="8">
-        <v>0</v>
-      </c>
+      <c r="B54" s="8"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
@@ -11092,7 +11084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -11389,8 +11381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79:B86"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11733,9 +11725,6 @@
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="B42">
-        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -12783,8 +12772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59:B66"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12887,9 +12876,6 @@
       <c r="A12" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -13040,9 +13026,6 @@
       <c r="A31" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
@@ -13186,9 +13169,6 @@
       <c r="A49" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="B49">
-        <v>0</v>
-      </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
@@ -13269,9 +13249,6 @@
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="B59">
-        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>